<commit_message>
Fixed the AUC scoring for models to work from probability, not rounded. Updated ALL
</commit_message>
<xml_diff>
--- a/nth_semester_graduation_prediction/ConfidenceIntervalResults/ALL.xlsx
+++ b/nth_semester_graduation_prediction/ConfidenceIntervalResults/ALL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>term</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>AUC Upper</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Acc.</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -368,43 +377,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -412,40 +438,61 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
       <c r="L2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
         <v>3</v>
       </c>
+      <c r="N2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -453,40 +500,61 @@
         <v>0.80407252440725197</v>
       </c>
       <c r="C3">
+        <v>0.83684895122705505</v>
+      </c>
+      <c r="D3">
         <v>0.86765986218138702</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.760522496371553</v>
       </c>
-      <c r="E3">
+      <c r="F3">
+        <v>0.79100145137880895</v>
+      </c>
+      <c r="G3">
         <v>0.82148040638606601</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.83541894852135801</v>
       </c>
-      <c r="G3">
+      <c r="I3">
+        <v>0.86335025196019499</v>
+      </c>
+      <c r="J3">
         <v>0.88944658944658905</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>0.76342525399129102</v>
       </c>
-      <c r="I3">
+      <c r="L3">
+        <v>0.79390420899854797</v>
+      </c>
+      <c r="M3">
         <v>0.82293178519593602</v>
       </c>
-      <c r="J3">
+      <c r="N3">
         <v>0.45652518213493798</v>
       </c>
-      <c r="K3">
+      <c r="O3">
+        <v>0.49795339191180399</v>
+      </c>
+      <c r="P3">
         <v>0.53992447964634305</v>
       </c>
-      <c r="L3">
+      <c r="Q3">
         <v>0.599419448476052</v>
       </c>
-      <c r="M3">
+      <c r="R3">
+        <v>0.63570391872278598</v>
+      </c>
+      <c r="S3">
         <v>0.67198838896952096</v>
       </c>
+      <c r="U3">
+        <v>689</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -494,40 +562,61 @@
         <v>0.84799595021142204</v>
       </c>
       <c r="C4">
+        <v>0.87889225682006</v>
+      </c>
+      <c r="D4">
         <v>0.90700615174299304</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.79140127388534998</v>
       </c>
-      <c r="E4">
+      <c r="F4">
+        <v>0.82165605095541405</v>
+      </c>
+      <c r="G4">
         <v>0.85191082802547702</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.85379352938381803</v>
       </c>
-      <c r="G4">
+      <c r="I4">
+        <v>0.88236069344770895</v>
+      </c>
+      <c r="J4">
         <v>0.90869899923017705</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>0.78662420382165599</v>
       </c>
-      <c r="I4">
+      <c r="L4">
+        <v>0.81687898089171895</v>
+      </c>
+      <c r="M4">
         <v>0.84713375796178303</v>
       </c>
-      <c r="J4">
+      <c r="N4">
         <v>0.45558597524501898</v>
       </c>
-      <c r="K4">
+      <c r="O4">
+        <v>0.49790935339715098</v>
+      </c>
+      <c r="P4">
         <v>0.54075324213892295</v>
       </c>
-      <c r="L4">
+      <c r="Q4">
         <v>0.65923566878980799</v>
       </c>
-      <c r="M4">
+      <c r="R4">
+        <v>0.69585987261146498</v>
+      </c>
+      <c r="S4">
         <v>0.73089171974522205</v>
       </c>
+      <c r="U4">
+        <v>628</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -535,40 +624,61 @@
         <v>0.80649717514124197</v>
       </c>
       <c r="C5">
+        <v>0.84855906750571997</v>
+      </c>
+      <c r="D5">
         <v>0.88678353978584901</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.80353982300884896</v>
       </c>
-      <c r="E5">
+      <c r="F5">
+        <v>0.83539823008849501</v>
+      </c>
+      <c r="G5">
         <v>0.86548672566371598</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.82432727272727202</v>
       </c>
-      <c r="G5">
+      <c r="I5">
+        <v>0.86037614416475905</v>
+      </c>
+      <c r="J5">
         <v>0.89400264738824897</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>0.79646017699115002</v>
       </c>
-      <c r="I5">
+      <c r="L5">
+        <v>0.82831858407079595</v>
+      </c>
+      <c r="M5">
         <v>0.86017699115044199</v>
       </c>
-      <c r="J5">
+      <c r="N5">
         <v>0.44194756554307102</v>
       </c>
-      <c r="K5">
+      <c r="O5">
+        <v>0.49576301487414098</v>
+      </c>
+      <c r="P5">
         <v>0.54811279350449804</v>
       </c>
-      <c r="L5">
+      <c r="Q5">
         <v>0.73805309734513203</v>
       </c>
-      <c r="M5">
+      <c r="R5">
+        <v>0.77345132743362799</v>
+      </c>
+      <c r="S5">
         <v>0.80707964601769899</v>
       </c>
+      <c r="U5">
+        <v>565</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -576,40 +686,61 @@
         <v>0.82253771073646798</v>
       </c>
       <c r="C6">
+        <v>0.86581046211587998</v>
+      </c>
+      <c r="D6">
         <v>0.90508308895405598</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.84427767354596595</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <v>0.87429643527204504</v>
+      </c>
+      <c r="G6">
         <v>0.90243902439024304</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.81770679286207204</v>
       </c>
-      <c r="G6">
+      <c r="I6">
+        <v>0.85925404644616399</v>
+      </c>
+      <c r="J6">
         <v>0.89664614937236398</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>0.83489681050656595</v>
       </c>
-      <c r="I6">
+      <c r="L6">
+        <v>0.86491557223264504</v>
+      </c>
+      <c r="M6">
         <v>0.89305816135084404</v>
       </c>
-      <c r="J6">
+      <c r="N6">
         <v>0.44049507329968701</v>
       </c>
-      <c r="K6">
+      <c r="O6">
+        <v>0.49387755102040798</v>
+      </c>
+      <c r="P6">
         <v>0.547625127681307</v>
       </c>
-      <c r="L6">
+      <c r="Q6">
         <v>0.78236397748592801</v>
       </c>
-      <c r="M6">
+      <c r="R6">
+        <v>0.81613508442776705</v>
+      </c>
+      <c r="S6">
         <v>0.84803001876172601</v>
       </c>
+      <c r="U6">
+        <v>533</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -617,40 +748,61 @@
         <v>0.74902177925433699</v>
       </c>
       <c r="C7">
+        <v>0.80497343013247502</v>
+      </c>
+      <c r="D7">
         <v>0.85563895304079995</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.83975659229208899</v>
       </c>
-      <c r="E7">
+      <c r="F7">
+        <v>0.87018255578093295</v>
+      </c>
+      <c r="G7">
         <v>0.89858012170385304</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.80435986159169504</v>
       </c>
-      <c r="G7">
+      <c r="I7">
+        <v>0.85199461118179698</v>
+      </c>
+      <c r="J7">
         <v>0.89585360377217205</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>0.85598377281947202</v>
       </c>
-      <c r="I7">
+      <c r="L7">
+        <v>0.884381338742393</v>
+      </c>
+      <c r="M7">
         <v>0.91075050709939098</v>
       </c>
-      <c r="J7">
+      <c r="N7">
         <v>0.42050691244239602</v>
       </c>
-      <c r="K7">
+      <c r="O7">
+        <v>0.49077539106354301</v>
+      </c>
+      <c r="P7">
         <v>0.556856591018831</v>
       </c>
-      <c r="L7">
+      <c r="Q7">
         <v>0.84381338742393497</v>
       </c>
-      <c r="M7">
+      <c r="R7">
+        <v>0.87423935091277805</v>
+      </c>
+      <c r="S7">
         <v>0.90263691683569902</v>
       </c>
+      <c r="U7">
+        <v>493</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -658,40 +810,61 @@
         <v>0.83558294209702599</v>
       </c>
       <c r="C8">
+        <v>0.88541232095675104</v>
+      </c>
+      <c r="D8">
         <v>0.92778301886792403</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.87552742616033696</v>
       </c>
-      <c r="E8">
+      <c r="F8">
+        <v>0.90295358649789004</v>
+      </c>
+      <c r="G8">
         <v>0.92827004219409204</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.83201243201243102</v>
       </c>
-      <c r="G8">
+      <c r="I8">
+        <v>0.88726649052055795</v>
+      </c>
+      <c r="J8">
         <v>0.93524645927391903</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>0.89662447257383904</v>
       </c>
-      <c r="I8">
+      <c r="L8">
+        <v>0.92194092827004204</v>
+      </c>
+      <c r="M8">
         <v>0.94514767932489396</v>
       </c>
-      <c r="J8">
+      <c r="N8">
         <v>0.413469387755102</v>
       </c>
-      <c r="K8">
+      <c r="O8">
+        <v>0.49170259120196502</v>
+      </c>
+      <c r="P8">
         <v>0.57066238647040401</v>
       </c>
-      <c r="L8">
+      <c r="Q8">
         <v>0.86497890295358604</v>
       </c>
-      <c r="M8">
+      <c r="R8">
+        <v>0.892405063291139</v>
+      </c>
+      <c r="S8">
         <v>0.91983122362869196</v>
       </c>
+      <c r="U8">
+        <v>474</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -699,40 +872,61 @@
         <v>0.85756416904329702</v>
       </c>
       <c r="C9">
+        <v>0.90392945544554404</v>
+      </c>
+      <c r="D9">
         <v>0.94259158009841404</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.88288288288288197</v>
       </c>
-      <c r="E9">
+      <c r="F9">
+        <v>0.90990990990990905</v>
+      </c>
+      <c r="G9">
         <v>0.93468468468468402</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>0.86417483660130701</v>
       </c>
-      <c r="G9">
+      <c r="I9">
+        <v>0.90798267326732596</v>
+      </c>
+      <c r="J9">
         <v>0.94662480376766001</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>0.89864864864864802</v>
       </c>
-      <c r="I9">
+      <c r="L9">
+        <v>0.92342342342342298</v>
+      </c>
+      <c r="M9">
         <v>0.94594594594594505</v>
       </c>
-      <c r="J9">
+      <c r="N9">
         <v>0.43120066472787699</v>
       </c>
-      <c r="K9">
+      <c r="O9">
+        <v>0.49900990099009901</v>
+      </c>
+      <c r="P9">
         <v>0.56143904994760696</v>
       </c>
-      <c r="L9">
+      <c r="Q9">
         <v>0.88288288288288197</v>
       </c>
-      <c r="M9">
+      <c r="R9">
+        <v>0.90990990990990905</v>
+      </c>
+      <c r="S9">
         <v>0.93693693693693603</v>
       </c>
+      <c r="U9">
+        <v>444</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -740,40 +934,61 @@
         <v>0.85244618395303295</v>
       </c>
       <c r="C10">
+        <v>0.90530925013683605</v>
+      </c>
+      <c r="D10">
         <v>0.94878762541806005</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.91400491400491402</v>
       </c>
-      <c r="E10">
+      <c r="F10">
+        <v>0.93857493857493801</v>
+      </c>
+      <c r="G10">
         <v>0.96068796068796003</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>0.80424566520823104</v>
       </c>
-      <c r="G10">
+      <c r="I10">
+        <v>0.87657361795292799</v>
+      </c>
+      <c r="J10">
         <v>0.93893705239351599</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>0.92383292383292304</v>
       </c>
-      <c r="I10">
+      <c r="L10">
+        <v>0.94594594594594505</v>
+      </c>
+      <c r="M10">
         <v>0.96805896805896796</v>
       </c>
-      <c r="J10">
+      <c r="N10">
         <v>0.39143844066123801</v>
       </c>
-      <c r="K10">
+      <c r="O10">
+        <v>0.48617952928297697</v>
+      </c>
+      <c r="P10">
         <v>0.58324210910417795</v>
       </c>
-      <c r="L10">
+      <c r="Q10">
         <v>0.90417690417690399</v>
       </c>
-      <c r="M10">
+      <c r="R10">
+        <v>0.92874692874692799</v>
+      </c>
+      <c r="S10">
         <v>0.95331695331695299</v>
       </c>
+      <c r="U10">
+        <v>407</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -781,40 +996,61 @@
         <v>0.83512544802867295</v>
       </c>
       <c r="C11">
+        <v>0.91582747482424398</v>
+      </c>
+      <c r="D11">
         <v>0.97036474164133701</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.91554054054054002</v>
       </c>
-      <c r="E11">
+      <c r="F11">
+        <v>0.94256756756756699</v>
+      </c>
+      <c r="G11">
         <v>0.96621621621621601</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>0.80889439625499104</v>
       </c>
-      <c r="G11">
+      <c r="I11">
+        <v>0.89891696750902494</v>
+      </c>
+      <c r="J11">
         <v>0.96532846715328402</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>0.92567567567567499</v>
       </c>
-      <c r="I11">
+      <c r="L11">
+        <v>0.95270270270270196</v>
+      </c>
+      <c r="M11">
         <v>0.97635135135135098</v>
       </c>
-      <c r="J11">
+      <c r="N11">
         <v>0.35824275362318803</v>
       </c>
-      <c r="K11">
+      <c r="O11">
+        <v>0.47814934448033403</v>
+      </c>
+      <c r="P11">
         <v>0.60260940472954605</v>
       </c>
-      <c r="L11">
+      <c r="Q11">
         <v>0.90540540540540504</v>
       </c>
-      <c r="M11">
+      <c r="R11">
+        <v>0.93581081081080997</v>
+      </c>
+      <c r="S11">
         <v>0.96283783783783705</v>
       </c>
+      <c r="U11">
+        <v>296</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -822,45 +1058,67 @@
         <v>0.45861204013377899</v>
       </c>
       <c r="C12">
+        <v>0.63468468468468398</v>
+      </c>
+      <c r="D12">
         <v>0.790977443609022</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.89847715736040601</v>
       </c>
-      <c r="E12">
+      <c r="F12">
+        <v>0.93401015228426398</v>
+      </c>
+      <c r="G12">
         <v>0.96446700507614203</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>0.52537080405932801</v>
       </c>
-      <c r="G12">
+      <c r="I12">
+        <v>0.74684684684684599</v>
+      </c>
+      <c r="J12">
         <v>0.94030732860520005</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>0.90355329949238505</v>
       </c>
-      <c r="I12">
-        <v>0.96954314720812096</v>
-      </c>
-      <c r="J12">
-        <v>0.29839968774394998</v>
-      </c>
-      <c r="K12">
-        <v>0.60050741608118596</v>
-      </c>
       <c r="L12">
-        <v>0.90355329949238505</v>
+        <v>0.93908629441624303</v>
       </c>
       <c r="M12">
         <v>0.96954314720812096</v>
+      </c>
+      <c r="N12">
+        <v>0.29839968774394998</v>
+      </c>
+      <c r="O12">
+        <v>0.44999999999999901</v>
+      </c>
+      <c r="P12">
+        <v>0.60050741608118596</v>
+      </c>
+      <c r="Q12">
+        <v>0.90355329949238505</v>
+      </c>
+      <c r="R12">
+        <v>0.93908629441624303</v>
+      </c>
+      <c r="S12">
+        <v>0.96954314720812096</v>
+      </c>
+      <c r="U12">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all AUCs and Accuracies.
</commit_message>
<xml_diff>
--- a/nth_semester_graduation_prediction/ConfidenceIntervalResults/ALL.xlsx
+++ b/nth_semester_graduation_prediction/ConfidenceIntervalResults/ALL.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="all" sheetId="1" r:id="rId1"/>
+    <sheet name="gbt" sheetId="2" r:id="rId2"/>
+    <sheet name="lr" sheetId="3" r:id="rId3"/>
+    <sheet name="zeror" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="12">
   <si>
     <t>term</t>
   </si>
@@ -57,6 +60,9 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -377,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U14" sqref="U2:U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,6 +1118,68 @@
         <v>197</v>
       </c>
     </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.86544508267602205</v>
+      </c>
+      <c r="C14">
+        <v>0.87839433555378699</v>
+      </c>
+      <c r="D14">
+        <v>0.89072171325872895</v>
+      </c>
+      <c r="E14">
+        <v>0.85907744392721097</v>
+      </c>
+      <c r="F14">
+        <v>0.86859923825645302</v>
+      </c>
+      <c r="G14">
+        <v>0.87812103258569596</v>
+      </c>
+      <c r="H14">
+        <v>0.88109434072109705</v>
+      </c>
+      <c r="I14">
+        <v>0.89275781599406001</v>
+      </c>
+      <c r="J14">
+        <v>0.90404135022313103</v>
+      </c>
+      <c r="K14">
+        <v>0.86309775708844605</v>
+      </c>
+      <c r="L14">
+        <v>0.87261955141768899</v>
+      </c>
+      <c r="M14">
+        <v>0.88214134574693104</v>
+      </c>
+      <c r="N14">
+        <v>0.67688727088314105</v>
+      </c>
+      <c r="O14">
+        <v>0.69526472016519802</v>
+      </c>
+      <c r="P14">
+        <v>0.71361829835490997</v>
+      </c>
+      <c r="Q14">
+        <v>0.80236986881083305</v>
+      </c>
+      <c r="R14">
+        <v>0.81358442657638597</v>
+      </c>
+      <c r="S14">
+        <v>0.82458738891239902</v>
+      </c>
+      <c r="U14">
+        <v>4726</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
@@ -1121,4 +1189,1000 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.80407252440725197</v>
+      </c>
+      <c r="C2">
+        <v>0.83684895122705505</v>
+      </c>
+      <c r="D2">
+        <v>0.86765986218138702</v>
+      </c>
+      <c r="E2">
+        <v>0.760522496371553</v>
+      </c>
+      <c r="F2">
+        <v>0.79100145137880895</v>
+      </c>
+      <c r="G2">
+        <v>0.82148040638606601</v>
+      </c>
+      <c r="I2">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.84799595021142204</v>
+      </c>
+      <c r="C3">
+        <v>0.87889225682006</v>
+      </c>
+      <c r="D3">
+        <v>0.90700615174299304</v>
+      </c>
+      <c r="E3">
+        <v>0.79140127388534998</v>
+      </c>
+      <c r="F3">
+        <v>0.82165605095541405</v>
+      </c>
+      <c r="G3">
+        <v>0.85191082802547702</v>
+      </c>
+      <c r="I3">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.80649717514124197</v>
+      </c>
+      <c r="C4">
+        <v>0.84855906750571997</v>
+      </c>
+      <c r="D4">
+        <v>0.88678353978584901</v>
+      </c>
+      <c r="E4">
+        <v>0.80353982300884896</v>
+      </c>
+      <c r="F4">
+        <v>0.83539823008849501</v>
+      </c>
+      <c r="G4">
+        <v>0.86548672566371598</v>
+      </c>
+      <c r="I4">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.82253771073646798</v>
+      </c>
+      <c r="C5">
+        <v>0.86581046211587998</v>
+      </c>
+      <c r="D5">
+        <v>0.90508308895405598</v>
+      </c>
+      <c r="E5">
+        <v>0.84427767354596595</v>
+      </c>
+      <c r="F5">
+        <v>0.87429643527204504</v>
+      </c>
+      <c r="G5">
+        <v>0.90243902439024304</v>
+      </c>
+      <c r="I5">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.74902177925433699</v>
+      </c>
+      <c r="C6">
+        <v>0.80497343013247502</v>
+      </c>
+      <c r="D6">
+        <v>0.85563895304079995</v>
+      </c>
+      <c r="E6">
+        <v>0.83975659229208899</v>
+      </c>
+      <c r="F6">
+        <v>0.87018255578093295</v>
+      </c>
+      <c r="G6">
+        <v>0.89858012170385304</v>
+      </c>
+      <c r="I6">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.83558294209702599</v>
+      </c>
+      <c r="C7">
+        <v>0.88541232095675104</v>
+      </c>
+      <c r="D7">
+        <v>0.92778301886792403</v>
+      </c>
+      <c r="E7">
+        <v>0.87552742616033696</v>
+      </c>
+      <c r="F7">
+        <v>0.90295358649789004</v>
+      </c>
+      <c r="G7">
+        <v>0.92827004219409204</v>
+      </c>
+      <c r="I7">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.85756416904329702</v>
+      </c>
+      <c r="C8">
+        <v>0.90392945544554404</v>
+      </c>
+      <c r="D8">
+        <v>0.94259158009841404</v>
+      </c>
+      <c r="E8">
+        <v>0.88288288288288197</v>
+      </c>
+      <c r="F8">
+        <v>0.90990990990990905</v>
+      </c>
+      <c r="G8">
+        <v>0.93468468468468402</v>
+      </c>
+      <c r="I8">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.85244618395303295</v>
+      </c>
+      <c r="C9">
+        <v>0.90530925013683605</v>
+      </c>
+      <c r="D9">
+        <v>0.94878762541806005</v>
+      </c>
+      <c r="E9">
+        <v>0.91400491400491402</v>
+      </c>
+      <c r="F9">
+        <v>0.93857493857493801</v>
+      </c>
+      <c r="G9">
+        <v>0.96068796068796003</v>
+      </c>
+      <c r="I9">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.83512544802867295</v>
+      </c>
+      <c r="C10">
+        <v>0.91582747482424398</v>
+      </c>
+      <c r="D10">
+        <v>0.97036474164133701</v>
+      </c>
+      <c r="E10">
+        <v>0.91554054054054002</v>
+      </c>
+      <c r="F10">
+        <v>0.94256756756756699</v>
+      </c>
+      <c r="G10">
+        <v>0.96621621621621601</v>
+      </c>
+      <c r="I10">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.45861204013377899</v>
+      </c>
+      <c r="C11">
+        <v>0.63468468468468398</v>
+      </c>
+      <c r="D11">
+        <v>0.790977443609022</v>
+      </c>
+      <c r="E11">
+        <v>0.89847715736040601</v>
+      </c>
+      <c r="F11">
+        <v>0.93401015228426398</v>
+      </c>
+      <c r="G11">
+        <v>0.96446700507614203</v>
+      </c>
+      <c r="I11">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.86544508267602205</v>
+      </c>
+      <c r="C13">
+        <v>0.87839433555378699</v>
+      </c>
+      <c r="D13">
+        <v>0.89072171325872895</v>
+      </c>
+      <c r="E13">
+        <v>0.85907744392721097</v>
+      </c>
+      <c r="F13">
+        <v>0.86859923825645302</v>
+      </c>
+      <c r="G13">
+        <v>0.87812103258569596</v>
+      </c>
+      <c r="I13">
+        <v>4726</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.83541894852135801</v>
+      </c>
+      <c r="C2">
+        <v>0.86335025196019499</v>
+      </c>
+      <c r="D2">
+        <v>0.88944658944658905</v>
+      </c>
+      <c r="E2">
+        <v>0.76342525399129102</v>
+      </c>
+      <c r="F2">
+        <v>0.79390420899854797</v>
+      </c>
+      <c r="G2">
+        <v>0.82293178519593602</v>
+      </c>
+      <c r="I2">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.85379352938381803</v>
+      </c>
+      <c r="C3">
+        <v>0.88236069344770895</v>
+      </c>
+      <c r="D3">
+        <v>0.90869899923017705</v>
+      </c>
+      <c r="E3">
+        <v>0.78662420382165599</v>
+      </c>
+      <c r="F3">
+        <v>0.81687898089171895</v>
+      </c>
+      <c r="G3">
+        <v>0.84713375796178303</v>
+      </c>
+      <c r="I3">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.82432727272727202</v>
+      </c>
+      <c r="C4">
+        <v>0.86037614416475905</v>
+      </c>
+      <c r="D4">
+        <v>0.89400264738824897</v>
+      </c>
+      <c r="E4">
+        <v>0.79646017699115002</v>
+      </c>
+      <c r="F4">
+        <v>0.82831858407079595</v>
+      </c>
+      <c r="G4">
+        <v>0.86017699115044199</v>
+      </c>
+      <c r="I4">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.81770679286207204</v>
+      </c>
+      <c r="C5">
+        <v>0.85925404644616399</v>
+      </c>
+      <c r="D5">
+        <v>0.89664614937236398</v>
+      </c>
+      <c r="E5">
+        <v>0.83489681050656595</v>
+      </c>
+      <c r="F5">
+        <v>0.86491557223264504</v>
+      </c>
+      <c r="G5">
+        <v>0.89305816135084404</v>
+      </c>
+      <c r="I5">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.80435986159169504</v>
+      </c>
+      <c r="C6">
+        <v>0.85199461118179698</v>
+      </c>
+      <c r="D6">
+        <v>0.89585360377217205</v>
+      </c>
+      <c r="E6">
+        <v>0.85598377281947202</v>
+      </c>
+      <c r="F6">
+        <v>0.884381338742393</v>
+      </c>
+      <c r="G6">
+        <v>0.91075050709939098</v>
+      </c>
+      <c r="I6">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.83201243201243102</v>
+      </c>
+      <c r="C7">
+        <v>0.88726649052055795</v>
+      </c>
+      <c r="D7">
+        <v>0.93524645927391903</v>
+      </c>
+      <c r="E7">
+        <v>0.89662447257383904</v>
+      </c>
+      <c r="F7">
+        <v>0.92194092827004204</v>
+      </c>
+      <c r="G7">
+        <v>0.94514767932489396</v>
+      </c>
+      <c r="I7">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.86417483660130701</v>
+      </c>
+      <c r="C8">
+        <v>0.90798267326732596</v>
+      </c>
+      <c r="D8">
+        <v>0.94662480376766001</v>
+      </c>
+      <c r="E8">
+        <v>0.89864864864864802</v>
+      </c>
+      <c r="F8">
+        <v>0.92342342342342298</v>
+      </c>
+      <c r="G8">
+        <v>0.94594594594594505</v>
+      </c>
+      <c r="I8">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.80424566520823104</v>
+      </c>
+      <c r="C9">
+        <v>0.87657361795292799</v>
+      </c>
+      <c r="D9">
+        <v>0.93893705239351599</v>
+      </c>
+      <c r="E9">
+        <v>0.92383292383292304</v>
+      </c>
+      <c r="F9">
+        <v>0.94594594594594505</v>
+      </c>
+      <c r="G9">
+        <v>0.96805896805896796</v>
+      </c>
+      <c r="I9">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.80889439625499104</v>
+      </c>
+      <c r="C10">
+        <v>0.89891696750902494</v>
+      </c>
+      <c r="D10">
+        <v>0.96532846715328402</v>
+      </c>
+      <c r="E10">
+        <v>0.92567567567567499</v>
+      </c>
+      <c r="F10">
+        <v>0.95270270270270196</v>
+      </c>
+      <c r="G10">
+        <v>0.97635135135135098</v>
+      </c>
+      <c r="I10">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.52537080405932801</v>
+      </c>
+      <c r="C11">
+        <v>0.74684684684684599</v>
+      </c>
+      <c r="D11">
+        <v>0.94030732860520005</v>
+      </c>
+      <c r="E11">
+        <v>0.90355329949238505</v>
+      </c>
+      <c r="F11">
+        <v>0.93908629441624303</v>
+      </c>
+      <c r="G11">
+        <v>0.96954314720812096</v>
+      </c>
+      <c r="I11">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.88109434072109705</v>
+      </c>
+      <c r="C13">
+        <v>0.89275781599406001</v>
+      </c>
+      <c r="D13">
+        <v>0.90404135022313103</v>
+      </c>
+      <c r="E13">
+        <v>0.86309775708844605</v>
+      </c>
+      <c r="F13">
+        <v>0.87261955141768899</v>
+      </c>
+      <c r="G13">
+        <v>0.88214134574693104</v>
+      </c>
+      <c r="I13">
+        <v>4726</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.45652518213493798</v>
+      </c>
+      <c r="C2">
+        <v>0.49795339191180399</v>
+      </c>
+      <c r="D2">
+        <v>0.53992447964634305</v>
+      </c>
+      <c r="E2">
+        <v>0.599419448476052</v>
+      </c>
+      <c r="F2">
+        <v>0.63570391872278598</v>
+      </c>
+      <c r="G2">
+        <v>0.67198838896952096</v>
+      </c>
+      <c r="I2">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.45558597524501898</v>
+      </c>
+      <c r="C3">
+        <v>0.49790935339715098</v>
+      </c>
+      <c r="D3">
+        <v>0.54075324213892295</v>
+      </c>
+      <c r="E3">
+        <v>0.65923566878980799</v>
+      </c>
+      <c r="F3">
+        <v>0.69585987261146498</v>
+      </c>
+      <c r="G3">
+        <v>0.73089171974522205</v>
+      </c>
+      <c r="I3">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.44194756554307102</v>
+      </c>
+      <c r="C4">
+        <v>0.49576301487414098</v>
+      </c>
+      <c r="D4">
+        <v>0.54811279350449804</v>
+      </c>
+      <c r="E4">
+        <v>0.73805309734513203</v>
+      </c>
+      <c r="F4">
+        <v>0.77345132743362799</v>
+      </c>
+      <c r="G4">
+        <v>0.80707964601769899</v>
+      </c>
+      <c r="I4">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.44049507329968701</v>
+      </c>
+      <c r="C5">
+        <v>0.49387755102040798</v>
+      </c>
+      <c r="D5">
+        <v>0.547625127681307</v>
+      </c>
+      <c r="E5">
+        <v>0.78236397748592801</v>
+      </c>
+      <c r="F5">
+        <v>0.81613508442776705</v>
+      </c>
+      <c r="G5">
+        <v>0.84803001876172601</v>
+      </c>
+      <c r="I5">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.42050691244239602</v>
+      </c>
+      <c r="C6">
+        <v>0.49077539106354301</v>
+      </c>
+      <c r="D6">
+        <v>0.556856591018831</v>
+      </c>
+      <c r="E6">
+        <v>0.84381338742393497</v>
+      </c>
+      <c r="F6">
+        <v>0.87423935091277805</v>
+      </c>
+      <c r="G6">
+        <v>0.90263691683569902</v>
+      </c>
+      <c r="I6">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.413469387755102</v>
+      </c>
+      <c r="C7">
+        <v>0.49170259120196502</v>
+      </c>
+      <c r="D7">
+        <v>0.57066238647040401</v>
+      </c>
+      <c r="E7">
+        <v>0.86497890295358604</v>
+      </c>
+      <c r="F7">
+        <v>0.892405063291139</v>
+      </c>
+      <c r="G7">
+        <v>0.91983122362869196</v>
+      </c>
+      <c r="I7">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.43120066472787699</v>
+      </c>
+      <c r="C8">
+        <v>0.49900990099009901</v>
+      </c>
+      <c r="D8">
+        <v>0.56143904994760696</v>
+      </c>
+      <c r="E8">
+        <v>0.88288288288288197</v>
+      </c>
+      <c r="F8">
+        <v>0.90990990990990905</v>
+      </c>
+      <c r="G8">
+        <v>0.93693693693693603</v>
+      </c>
+      <c r="I8">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.39143844066123801</v>
+      </c>
+      <c r="C9">
+        <v>0.48617952928297697</v>
+      </c>
+      <c r="D9">
+        <v>0.58324210910417795</v>
+      </c>
+      <c r="E9">
+        <v>0.90417690417690399</v>
+      </c>
+      <c r="F9">
+        <v>0.92874692874692799</v>
+      </c>
+      <c r="G9">
+        <v>0.95331695331695299</v>
+      </c>
+      <c r="I9">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.35824275362318803</v>
+      </c>
+      <c r="C10">
+        <v>0.47814934448033403</v>
+      </c>
+      <c r="D10">
+        <v>0.60260940472954605</v>
+      </c>
+      <c r="E10">
+        <v>0.90540540540540504</v>
+      </c>
+      <c r="F10">
+        <v>0.93581081081080997</v>
+      </c>
+      <c r="G10">
+        <v>0.96283783783783705</v>
+      </c>
+      <c r="I10">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.29839968774394998</v>
+      </c>
+      <c r="C11">
+        <v>0.44999999999999901</v>
+      </c>
+      <c r="D11">
+        <v>0.60050741608118596</v>
+      </c>
+      <c r="E11">
+        <v>0.90355329949238505</v>
+      </c>
+      <c r="F11">
+        <v>0.93908629441624303</v>
+      </c>
+      <c r="G11">
+        <v>0.96954314720812096</v>
+      </c>
+      <c r="I11">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.67688727088314105</v>
+      </c>
+      <c r="C13">
+        <v>0.69526472016519802</v>
+      </c>
+      <c r="D13">
+        <v>0.71361829835490997</v>
+      </c>
+      <c r="E13">
+        <v>0.80236986881083305</v>
+      </c>
+      <c r="F13">
+        <v>0.81358442657638597</v>
+      </c>
+      <c r="G13">
+        <v>0.82458738891239902</v>
+      </c>
+      <c r="I13">
+        <v>4726</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added graphs for grad prediction performance.
</commit_message>
<xml_diff>
--- a/nth_semester_graduation_prediction/ConfidenceIntervalResults/ALL.xlsx
+++ b/nth_semester_graduation_prediction/ConfidenceIntervalResults/ALL.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
-    <sheet name="gbt" sheetId="2" r:id="rId2"/>
-    <sheet name="lr" sheetId="3" r:id="rId3"/>
-    <sheet name="zeror" sheetId="4" r:id="rId4"/>
+    <sheet name="graphing" sheetId="5" r:id="rId2"/>
+    <sheet name="gbt" sheetId="2" r:id="rId3"/>
+    <sheet name="lr" sheetId="3" r:id="rId4"/>
+    <sheet name="zeror" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="15">
   <si>
     <t>term</t>
   </si>
@@ -63,6 +64,15 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>ZeroR (Most Frequent)</t>
+  </si>
+  <si>
+    <t>Gradient Boosted Trees</t>
+  </si>
+  <si>
+    <t>auc</t>
   </si>
 </sst>
 </file>
@@ -118,6 +128,2524 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Model Performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> for Predicting a Student's Graduation Status</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0873455745416137E-2"/>
+          <c:y val="0.10892799661082168"/>
+          <c:w val="0.89034720405601486"/>
+          <c:h val="0.73357349262964722"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-7808-4790-BEC7-312FBCCFC63A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7808-4790-BEC7-312FBCCFC63A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>graphing!$B$4:$D$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>1.2327377704941966E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1283534229071024E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.835357818971195E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>graphing!$B$3:$D$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>1.2949252877764938E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1663475272962964E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.8377449282056979E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="sq" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>graphing!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gradient Boosted Trees</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ZeroR (Most Frequent)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graphing!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.87839433555378699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89275781599406001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69526472016519802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7808-4790-BEC7-312FBCCFC63A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="406436072"/>
+        <c:axId val="406440336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="406436072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Predctive Model</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45278460891077799"/>
+              <c:y val="0.92753527084124765"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406440336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="406440336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>AUC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.4437564742221287E-3"/>
+              <c:y val="0.43144111985529759"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406436072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1" cap="none" spc="0">
+                <a:ln w="0"/>
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="dk1">
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </a:rPr>
+              <a:t>Model Performance for Predicting a Student's Graduation Status by</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1" cap="none" spc="0" baseline="0">
+                <a:ln w="0"/>
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="dk1">
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </a:rPr>
+              <a:t> Term</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400" b="1" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphing!$B$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gradient Boosted Trees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>graphing!$A$35:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graphing!$B$35:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.83684895122705505</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87889225682006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84855906750571997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86581046211587998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80497343013247502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88541232095675104</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90392945544554404</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.90530925013683605</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91582747482424398</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.63468468468468398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94F9-4DA7-9EDA-278723FB1DA4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphing!$C$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Logistic Regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>graphing!$A$35:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graphing!$C$35:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.86335025196019499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88236069344770895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86037614416475905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85925404644616399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85199461118179698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88726649052055795</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90798267326732596</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87657361795292799</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89891696750902494</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.74684684684684599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-94F9-4DA7-9EDA-278723FB1DA4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphing!$D$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ZeroR (Most Frequent)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>graphing!$A$35:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>graphing!$D$35:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.49795339191180399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49790935339715098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49576301487414098</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49387755102040798</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.49077539106354301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.49170259120196502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.49900990099009901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48617952928297697</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47814934448033403</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.44999999999999901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-94F9-4DA7-9EDA-278723FB1DA4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="480874320"/>
+        <c:axId val="480875960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="480874320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Term Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44699509479413113"/>
+              <c:y val="0.87669583496646231"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="480875960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="480875960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>AUC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.7838499011852122E-3"/>
+              <c:y val="0.40550932322291117"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="480874320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9575">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" cap="all" spc="0" baseline="0">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>40821</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>394607</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>136073</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,7 +2914,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U14" sqref="U2:U14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,10 +3721,245 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF55" sqref="AF55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0.87839433555378699</v>
+      </c>
+      <c r="C2">
+        <v>0.89275781599406001</v>
+      </c>
+      <c r="D2">
+        <v>0.69526472016519802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1.2949252877764938E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.1663475272962964E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.8377449282056979E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1.2327377704941966E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.1283534229071024E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.835357818971195E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>0.83684895122705505</v>
+      </c>
+      <c r="C35">
+        <v>0.86335025196019499</v>
+      </c>
+      <c r="D35">
+        <v>0.49795339191180399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>0.87889225682006</v>
+      </c>
+      <c r="C36">
+        <v>0.88236069344770895</v>
+      </c>
+      <c r="D36">
+        <v>0.49790935339715098</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>0.84855906750571997</v>
+      </c>
+      <c r="C37">
+        <v>0.86037614416475905</v>
+      </c>
+      <c r="D37">
+        <v>0.49576301487414098</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>0.86581046211587998</v>
+      </c>
+      <c r="C38">
+        <v>0.85925404644616399</v>
+      </c>
+      <c r="D38">
+        <v>0.49387755102040798</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>0.80497343013247502</v>
+      </c>
+      <c r="C39">
+        <v>0.85199461118179698</v>
+      </c>
+      <c r="D39">
+        <v>0.49077539106354301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>0.88541232095675104</v>
+      </c>
+      <c r="C40">
+        <v>0.88726649052055795</v>
+      </c>
+      <c r="D40">
+        <v>0.49170259120196502</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>0.90392945544554404</v>
+      </c>
+      <c r="C41">
+        <v>0.90798267326732596</v>
+      </c>
+      <c r="D41">
+        <v>0.49900990099009901</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>0.90530925013683605</v>
+      </c>
+      <c r="C42">
+        <v>0.87657361795292799</v>
+      </c>
+      <c r="D42">
+        <v>0.48617952928297697</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>0.91582747482424398</v>
+      </c>
+      <c r="C43">
+        <v>0.89891696750902494</v>
+      </c>
+      <c r="D43">
+        <v>0.47814934448033403</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>0.63468468468468398</v>
+      </c>
+      <c r="C44">
+        <v>0.74684684684684599</v>
+      </c>
+      <c r="D44">
+        <v>0.44999999999999901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I13"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,12 +4286,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I13"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,12 +4618,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>